<commit_message>
問い合わせ履歴 随時対応 Signed-off-by: LiuYiYang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_物件管理_車室一覧.xlsx
+++ b/test_物件管理/test_物件管理_車室一覧.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6387" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6391" uniqueCount="532">
   <si>
     <t>URL:</t>
   </si>
@@ -1853,6 +1853,145 @@
   </si>
   <si>
     <t>//*[@id="parkingposition_form"]/div/div[2]/div[1]/a</t>
+  </si>
+  <si>
+    <t>EXPECT_003</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>001-002-005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>001-002-002</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>車室複数追加</t>
+  </si>
+  <si>
+    <t>001-002-001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>001-002-003</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>001-002-004</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IN_FORM_006</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EXPECT_006</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RESULT_006</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>001-002-006</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IN_FORM_005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EXPECT_005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RESULT_005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IN_DB_003</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SELECT id,created_date,updated_date,is_deleted,deleted_date,name,price_recruitment,price_recruitment_no_tax,price_homepage,price_homepage_no_tax,price_handbill,price_handbill_no_tax,length,width,height,weight,tyre_width,tyre_width_ap,min_height,min_height_ap,f_value,r_value,parking_lot_id,category_id,is_lock,lock_content_type_id,lock_object_id,lock_reason,sublease_cost,sublease_cost_no_tax,category_comment,entering_method FROM ap_parking_position WHERE 1=1  LIMIT 100</t>
+  </si>
+  <si>
+    <t>100001</t>
+  </si>
+  <si>
+    <t>SELECT id,created_date,updated_date,is_deleted,deleted_date,comment,parking_position_id FROM ap_parking_position_comment WHERE 1=1  LIMIT 100</t>
+  </si>
+  <si>
+    <t>SELECT id,created_date,updated_date,is_deleted,deleted_date,category,key_count,comment,parking_position_id,password,model_no,reissue_cost FROM ap_parking_position_key WHERE 1=1  LIMIT 100</t>
+  </si>
+  <si>
+    <t>SHOT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLICK</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE FROM ap_parking_lot_image;</t>
+  </si>
+  <si>
+    <t>SET FOREIGN_KEY_CHECKS=0;</t>
+  </si>
+  <si>
+    <t>SET FOREIGN_KEY_CHECKS=1;</t>
+  </si>
+  <si>
+    <t>TRUNCATE TABLE ap_parking_position;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRUNCATE TABLE ap_parking_position_key;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRUNCATE TABLE ap_parking_position_comment;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRUNCATE TABLE ap_parking_position_cancellation;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-05-08 08:58:20</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>/html/body/main/div/div/div/div/form/div/button</t>
+  </si>
+  <si>
+    <r>
+      <t>車室</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>删</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>除后</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1888,116 +2027,7 @@
       </rPr>
       <t>确认</t>
     </r>
-  </si>
-  <si>
-    <t>EXPECT_003</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>001-002-005</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>001-002-002</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>車室複数追加</t>
-  </si>
-  <si>
-    <t>001-002-001</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>001-002-003</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>001-002-004</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IN_FORM_006</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>EXPECT_006</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>RESULT_006</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>001-002-006</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IN_FORM_005</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>EXPECT_005</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>RESULT_005</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IN_DB_003</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SELECT id,created_date,updated_date,is_deleted,deleted_date,name,price_recruitment,price_recruitment_no_tax,price_homepage,price_homepage_no_tax,price_handbill,price_handbill_no_tax,length,width,height,weight,tyre_width,tyre_width_ap,min_height,min_height_ap,f_value,r_value,parking_lot_id,category_id,is_lock,lock_content_type_id,lock_object_id,lock_reason,sublease_cost,sublease_cost_no_tax,category_comment,entering_method FROM ap_parking_position WHERE 1=1  LIMIT 100</t>
-  </si>
-  <si>
-    <t>100001</t>
-  </si>
-  <si>
-    <t>SELECT id,created_date,updated_date,is_deleted,deleted_date,comment,parking_position_id FROM ap_parking_position_comment WHERE 1=1  LIMIT 100</t>
-  </si>
-  <si>
-    <t>SELECT id,created_date,updated_date,is_deleted,deleted_date,category,key_count,comment,parking_position_id,password,model_no,reissue_cost FROM ap_parking_position_key WHERE 1=1  LIMIT 100</t>
-  </si>
-  <si>
-    <t>SHOT</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CLICK</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DELETE FROM ap_parking_lot_image;</t>
-  </si>
-  <si>
-    <t>SET FOREIGN_KEY_CHECKS=0;</t>
-  </si>
-  <si>
-    <t>SET FOREIGN_KEY_CHECKS=1;</t>
-  </si>
-  <si>
-    <t>TRUNCATE TABLE ap_parking_position;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRUNCATE TABLE ap_parking_position_key;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRUNCATE TABLE ap_parking_position_comment;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRUNCATE TABLE ap_parking_position_cancellation;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2018-05-08 08:58:20</t>
-  </si>
-  <si>
-    <t>-1</t>
   </si>
 </sst>
 </file>
@@ -3067,7 +3097,7 @@
         <v>253</v>
       </c>
       <c r="B1" s="128" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" spans="1:75" ht="14.25">
@@ -3075,7 +3105,7 @@
         <v>253</v>
       </c>
       <c r="B2" s="131" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
@@ -3155,7 +3185,7 @@
         <v>253</v>
       </c>
       <c r="B3" s="131" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="42"/>
@@ -3234,7 +3264,7 @@
         <v>253</v>
       </c>
       <c r="B4" s="131" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="44"/>
@@ -3314,7 +3344,7 @@
         <v>253</v>
       </c>
       <c r="B5" s="131" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
@@ -3394,7 +3424,7 @@
         <v>253</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C6" s="44"/>
       <c r="D6" s="44"/>
@@ -3562,7 +3592,7 @@
         <v>253</v>
       </c>
       <c r="B9" s="129" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="10" spans="1:75" ht="14.25">
@@ -5837,7 +5867,7 @@
     </row>
     <row r="16" spans="1:4" ht="14.25">
       <c r="A16" s="91" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B16" s="84" t="s">
         <v>472</v>
@@ -5847,7 +5877,7 @@
     </row>
     <row r="17" spans="1:4" ht="14.25">
       <c r="A17" s="91" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B17" s="84" t="s">
         <v>485</v>
@@ -9044,8 +9074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9074,12 +9104,26 @@
         <v>433</v>
       </c>
       <c r="B4" s="92" t="s">
-        <v>499</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="84" customFormat="1"/>
-    <row r="6" spans="1:9" s="84" customFormat="1"/>
-    <row r="7" spans="1:9" s="84" customFormat="1"/>
+    <row r="6" spans="1:9" s="84" customFormat="1" ht="14.25">
+      <c r="A6" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="84" customFormat="1" ht="14.25">
+      <c r="A7" s="91" t="s">
+        <v>433</v>
+      </c>
+      <c r="B7" s="92" t="s">
+        <v>530</v>
+      </c>
+    </row>
     <row r="8" spans="1:9" s="84" customFormat="1"/>
     <row r="9" spans="1:9" s="84" customFormat="1"/>
     <row r="10" spans="1:9" s="84" customFormat="1"/>
@@ -11968,7 +12012,7 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="89" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>408</v>
@@ -11988,7 +12032,7 @@
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="89" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>244</v>
@@ -12000,21 +12044,21 @@
         <v>246</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="22" customFormat="1">
       <c r="B7" s="89" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C7" s="89" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>461</v>
       </c>
       <c r="E7" s="89" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F7" s="89" t="s">
         <v>483</v>
@@ -12026,14 +12070,14 @@
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="89" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C8" s="89"/>
       <c r="D8" s="89" t="s">
         <v>481</v>
       </c>
       <c r="E8" s="89" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F8" s="89" t="s">
         <v>482</v>
@@ -12044,17 +12088,17 @@
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="89" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C9" s="89"/>
       <c r="D9" s="89" t="s">
+        <v>510</v>
+      </c>
+      <c r="E9" s="89" t="s">
         <v>511</v>
       </c>
-      <c r="E9" s="89" t="s">
+      <c r="F9" s="89" t="s">
         <v>512</v>
-      </c>
-      <c r="F9" s="89" t="s">
-        <v>513</v>
       </c>
       <c r="I9" s="22" t="s">
         <v>460</v>
@@ -12062,16 +12106,16 @@
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="89" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D10" s="89" t="s">
+        <v>506</v>
+      </c>
+      <c r="E10" s="89" t="s">
         <v>507</v>
       </c>
-      <c r="E10" s="89" t="s">
+      <c r="F10" s="89" t="s">
         <v>508</v>
-      </c>
-      <c r="F10" s="89" t="s">
-        <v>509</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>458</v>
@@ -17624,7 +17668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BW54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -17766,7 +17810,7 @@
         <v>264</v>
       </c>
       <c r="G5" s="118" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H5" s="118" t="s">
         <v>214</v>
@@ -20880,10 +20924,10 @@
         <v>412</v>
       </c>
       <c r="C53" s="139" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D53" s="139" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E53" s="139" t="s">
         <v>79</v>
@@ -20910,7 +20954,7 @@
         <v>121</v>
       </c>
       <c r="M53" s="139" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="N53" s="140"/>
       <c r="O53" s="140"/>
@@ -21321,7 +21365,7 @@
         <v>253</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C6" s="113"/>
       <c r="D6" s="113"/>
@@ -24527,7 +24571,7 @@
     <row r="38" spans="1:74">
       <c r="A38" s="111"/>
       <c r="B38" s="114" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C38" s="115" t="s">
         <v>89</v>
@@ -24682,7 +24726,7 @@
         <v>264</v>
       </c>
       <c r="G40" s="109" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H40" s="109" t="s">
         <v>214</v>
@@ -25271,7 +25315,7 @@
     <row r="48" spans="1:74">
       <c r="A48" s="105"/>
       <c r="B48" s="114" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C48" s="116"/>
       <c r="D48" s="116"/>
@@ -25521,7 +25565,7 @@
     <row r="58" spans="1:33">
       <c r="A58" s="105"/>
       <c r="B58" s="114" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C58" s="116"/>
       <c r="D58" s="116"/>

</xml_diff>

<commit_message>
start update 、値上げ更新 Signed-off-by: LiuYiYang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_物件管理_車室一覧.xlsx
+++ b/test_物件管理/test_物件管理_車室一覧.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6524" uniqueCount="564">
   <si>
     <t>URL:</t>
   </si>
@@ -1945,12 +1945,6 @@
   <si>
     <t>TRUNCATE TABLE ap_parking_position_comment;</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2018-05-08 08:58:20</t>
-  </si>
-  <si>
-    <t>-1</t>
   </si>
   <si>
     <t>/html/body/main/div/div/div/div/form/div/button</t>
@@ -2123,6 +2117,14 @@
   </si>
   <si>
     <t>5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2517,7 +2519,7 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2871,6 +2873,40 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="ハイパーリンク 2" xfId="11"/>
@@ -3205,7 +3241,7 @@
         <v>253</v>
       </c>
       <c r="B1" s="142" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
@@ -3213,7 +3249,7 @@
         <v>253</v>
       </c>
       <c r="B2" s="142" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
@@ -3221,7 +3257,7 @@
         <v>253</v>
       </c>
       <c r="B3" s="142" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
@@ -3229,7 +3265,7 @@
         <v>253</v>
       </c>
       <c r="B4" s="141" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25">
@@ -3237,7 +3273,7 @@
         <v>253</v>
       </c>
       <c r="B5" s="142" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25">
@@ -3245,7 +3281,7 @@
         <v>253</v>
       </c>
       <c r="B6" s="142" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25">
@@ -3253,7 +3289,7 @@
         <v>253</v>
       </c>
       <c r="B7" s="142" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25">
@@ -3269,7 +3305,7 @@
         <v>253</v>
       </c>
       <c r="B9" s="142" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25">
@@ -3277,7 +3313,7 @@
         <v>253</v>
       </c>
       <c r="B10" s="142" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25">
@@ -3285,7 +3321,7 @@
         <v>253</v>
       </c>
       <c r="B11" s="142" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.25">
@@ -3293,7 +3329,7 @@
         <v>253</v>
       </c>
       <c r="B12" s="142" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25">
@@ -3301,7 +3337,7 @@
         <v>253</v>
       </c>
       <c r="B13" s="142" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.25">
@@ -3325,7 +3361,7 @@
         <v>253</v>
       </c>
       <c r="B16" s="142" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="17" spans="1:75" ht="14.25">
@@ -3333,7 +3369,7 @@
         <v>253</v>
       </c>
       <c r="B17" s="142" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="18" spans="1:75" ht="14.25">
@@ -3349,7 +3385,7 @@
         <v>253</v>
       </c>
       <c r="B19" s="142" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:75" ht="14.25">
@@ -3357,7 +3393,7 @@
         <v>253</v>
       </c>
       <c r="B20" s="142" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="21" spans="1:75" ht="14.25">
@@ -3365,7 +3401,7 @@
         <v>253</v>
       </c>
       <c r="B21" s="142" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="22" spans="1:75" ht="14.25">
@@ -3373,7 +3409,7 @@
         <v>253</v>
       </c>
       <c r="B22" s="142" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="23" spans="1:75" ht="14.25">
@@ -3381,7 +3417,7 @@
         <v>253</v>
       </c>
       <c r="B23" s="142" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="24" spans="1:75" ht="14.25">
@@ -3389,7 +3425,7 @@
         <v>253</v>
       </c>
       <c r="B24" s="142" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="25" spans="1:75" ht="14.25">
@@ -3405,7 +3441,7 @@
         <v>253</v>
       </c>
       <c r="B26" s="142" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="27" spans="1:75" ht="14.25">
@@ -3413,7 +3449,7 @@
         <v>253</v>
       </c>
       <c r="B27" s="142" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="28" spans="1:75" ht="14.25">
@@ -3421,7 +3457,7 @@
         <v>253</v>
       </c>
       <c r="B28" s="142" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="29" spans="1:75" ht="14.25">
@@ -3429,7 +3465,7 @@
         <v>253</v>
       </c>
       <c r="B29" s="142" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="30" spans="1:75" ht="14.25">
@@ -3437,7 +3473,7 @@
         <v>253</v>
       </c>
       <c r="B30" s="142" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C30" s="141"/>
       <c r="D30" s="141"/>
@@ -3518,7 +3554,7 @@
         <v>253</v>
       </c>
       <c r="B31" s="142" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C31" s="141"/>
       <c r="D31" s="141"/>
@@ -3599,7 +3635,7 @@
         <v>253</v>
       </c>
       <c r="B32" s="142" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C32" s="141"/>
       <c r="D32" s="141"/>
@@ -3680,7 +3716,7 @@
         <v>253</v>
       </c>
       <c r="B33" s="142" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C33" s="141"/>
       <c r="D33" s="141"/>
@@ -3761,7 +3797,7 @@
         <v>253</v>
       </c>
       <c r="B34" s="142" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C34" s="141"/>
       <c r="D34" s="141"/>
@@ -3842,7 +3878,7 @@
         <v>253</v>
       </c>
       <c r="B35" s="142" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C35" s="141"/>
       <c r="D35" s="141"/>
@@ -3923,7 +3959,7 @@
         <v>253</v>
       </c>
       <c r="B36" s="142" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C36" s="141"/>
       <c r="D36" s="141"/>
@@ -4004,7 +4040,7 @@
         <v>253</v>
       </c>
       <c r="B37" s="142" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C37" s="141"/>
       <c r="D37" s="141"/>
@@ -4085,7 +4121,7 @@
         <v>253</v>
       </c>
       <c r="B38" s="142" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C38" s="141"/>
       <c r="D38" s="141"/>
@@ -5646,7 +5682,7 @@
         <v>264</v>
       </c>
       <c r="BU54" s="143" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="BV54" s="40">
         <v>1</v>
@@ -5864,7 +5900,7 @@
         <v>264</v>
       </c>
       <c r="BU55" s="143" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="BV55" s="40">
         <v>1</v>
@@ -6082,7 +6118,7 @@
         <v>264</v>
       </c>
       <c r="BU56" s="143" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="BV56" s="40">
         <v>1</v>
@@ -6901,10 +6937,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BV51"/>
+  <dimension ref="A1:BW56"/>
   <sheetViews>
-    <sheetView topLeftCell="AX4" workbookViewId="0">
-      <selection activeCell="BU14" sqref="BU14:BU19"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8638,7 +8674,7 @@
         <v>264</v>
       </c>
       <c r="BU16" s="143" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="BV16" s="88">
         <v>1</v>
@@ -8860,7 +8896,7 @@
         <v>264</v>
       </c>
       <c r="BU17" s="143" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="BV17" s="88">
         <v>1</v>
@@ -9082,7 +9118,7 @@
         <v>264</v>
       </c>
       <c r="BU18" s="143" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="BV18" s="88">
         <v>1</v>
@@ -9653,7 +9689,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
+    <row r="33" spans="1:74" s="84" customFormat="1" ht="12.75" customHeight="1">
       <c r="A33" s="95"/>
       <c r="B33" s="88" t="s">
         <v>239</v>
@@ -9677,382 +9713,868 @@
         <v>264</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
+    <row r="34" spans="1:74" s="84" customFormat="1" ht="12.75" customHeight="1">
       <c r="B34" s="93"/>
       <c r="C34" s="93"/>
     </row>
-    <row r="35" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A35" s="94" t="s">
+    <row r="35" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A35" s="158" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="95" t="s">
+      <c r="B35" s="156" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B36" s="96" t="s">
+    <row r="36" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B36" s="152" t="s">
         <v>442</v>
       </c>
-      <c r="C36" s="97" t="s">
+      <c r="C36" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="97" t="s">
+      <c r="D36" s="115" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B37" s="87" t="s">
+    <row r="37" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B37" s="150" t="s">
         <v>413</v>
       </c>
-      <c r="C37" s="86" t="s">
+      <c r="C37" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="86" t="s">
+      <c r="D37" s="149" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="86" t="s">
+      <c r="E37" s="149" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="86" t="s">
+      <c r="F37" s="149" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="86" t="s">
+      <c r="G37" s="149" t="s">
         <v>119</v>
       </c>
-      <c r="H37" s="86" t="s">
+      <c r="H37" s="149" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B38" s="88" t="s">
+    <row r="38" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B38" s="157" t="s">
         <v>416</v>
       </c>
-      <c r="C38" s="88" t="s">
+      <c r="C38" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="D38" s="88" t="s">
+      <c r="D38" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="E38" s="88" t="s">
+      <c r="E38" s="157" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G38" s="88" t="s">
+      <c r="F38" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G38" s="157" t="s">
         <v>373</v>
       </c>
-      <c r="H38" s="88" t="s">
+      <c r="H38" s="157" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B39" s="88" t="s">
+    <row r="39" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B39" s="157" t="s">
         <v>417</v>
       </c>
-      <c r="C39" s="88" t="s">
+      <c r="C39" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="D39" s="88" t="s">
+      <c r="D39" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="E39" s="88" t="s">
+      <c r="E39" s="157" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G39" s="88" t="s">
+      <c r="F39" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G39" s="157" t="s">
         <v>373</v>
       </c>
-      <c r="H39" s="88" t="s">
+      <c r="H39" s="157" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B40" s="88" t="s">
+    <row r="40" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A40" s="155"/>
+      <c r="B40" s="157" t="s">
         <v>404</v>
       </c>
-      <c r="C40" s="88" t="s">
+      <c r="C40" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="D40" s="88" t="s">
+      <c r="D40" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="E40" s="88" t="s">
+      <c r="E40" s="157" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G40" s="88" t="s">
+      <c r="F40" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G40" s="157" t="s">
+        <v>373</v>
+      </c>
+      <c r="H40" s="157" t="s">
+        <v>417</v>
+      </c>
+      <c r="I40" s="155"/>
+      <c r="J40" s="155"/>
+      <c r="K40" s="155"/>
+      <c r="L40" s="155"/>
+      <c r="M40" s="155"/>
+      <c r="N40" s="155"/>
+      <c r="O40" s="155"/>
+      <c r="P40" s="155"/>
+      <c r="Q40" s="155"/>
+      <c r="R40" s="155"/>
+      <c r="S40" s="155"/>
+      <c r="T40" s="155"/>
+      <c r="U40" s="155"/>
+      <c r="V40" s="155"/>
+      <c r="W40" s="155"/>
+      <c r="X40" s="155"/>
+      <c r="Y40" s="155"/>
+      <c r="Z40" s="155"/>
+      <c r="AA40" s="155"/>
+      <c r="AB40" s="155"/>
+      <c r="AC40" s="155"/>
+      <c r="AD40" s="155"/>
+      <c r="AE40" s="155"/>
+      <c r="AF40" s="155"/>
+      <c r="AG40" s="155"/>
+      <c r="AH40" s="155"/>
+      <c r="AI40" s="155"/>
+      <c r="AJ40" s="155"/>
+      <c r="AK40" s="155"/>
+      <c r="AL40" s="155"/>
+      <c r="AM40" s="155"/>
+      <c r="AN40" s="155"/>
+      <c r="AO40" s="155"/>
+      <c r="AP40" s="155"/>
+      <c r="AQ40" s="155"/>
+      <c r="AR40" s="155"/>
+      <c r="AS40" s="155"/>
+      <c r="AT40" s="155"/>
+      <c r="AU40" s="155"/>
+      <c r="AV40" s="155"/>
+      <c r="AW40" s="155"/>
+      <c r="AX40" s="155"/>
+      <c r="AY40" s="155"/>
+      <c r="AZ40" s="155"/>
+      <c r="BA40" s="155"/>
+      <c r="BB40" s="155"/>
+      <c r="BC40" s="155"/>
+      <c r="BD40" s="155"/>
+      <c r="BE40" s="155"/>
+      <c r="BF40" s="155"/>
+      <c r="BG40" s="155"/>
+      <c r="BH40" s="155"/>
+      <c r="BI40" s="155"/>
+      <c r="BJ40" s="155"/>
+      <c r="BK40" s="155"/>
+      <c r="BL40" s="155"/>
+      <c r="BM40" s="155"/>
+      <c r="BN40" s="155"/>
+      <c r="BO40" s="155"/>
+      <c r="BP40" s="155"/>
+      <c r="BQ40" s="155"/>
+      <c r="BR40" s="155"/>
+      <c r="BS40" s="155"/>
+      <c r="BT40" s="155"/>
+      <c r="BU40" s="155"/>
+      <c r="BV40" s="155"/>
+    </row>
+    <row r="41" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A41" s="155"/>
+      <c r="B41" s="157" t="s">
+        <v>422</v>
+      </c>
+      <c r="C41" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D41" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E41" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G41" s="157" t="s">
         <v>374</v>
       </c>
-      <c r="H40" s="88" t="s">
+      <c r="H41" s="157" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B41" s="88" t="s">
+      <c r="I41" s="155"/>
+      <c r="J41" s="155"/>
+      <c r="K41" s="155"/>
+      <c r="L41" s="155"/>
+      <c r="M41" s="155"/>
+      <c r="N41" s="155"/>
+      <c r="O41" s="155"/>
+      <c r="P41" s="155"/>
+      <c r="Q41" s="155"/>
+      <c r="R41" s="155"/>
+      <c r="S41" s="155"/>
+      <c r="T41" s="155"/>
+      <c r="U41" s="155"/>
+      <c r="V41" s="155"/>
+      <c r="W41" s="155"/>
+      <c r="X41" s="155"/>
+      <c r="Y41" s="155"/>
+      <c r="Z41" s="155"/>
+      <c r="AA41" s="155"/>
+      <c r="AB41" s="155"/>
+      <c r="AC41" s="155"/>
+      <c r="AD41" s="155"/>
+      <c r="AE41" s="155"/>
+      <c r="AF41" s="155"/>
+      <c r="AG41" s="155"/>
+      <c r="AH41" s="155"/>
+      <c r="AI41" s="155"/>
+      <c r="AJ41" s="155"/>
+      <c r="AK41" s="155"/>
+      <c r="AL41" s="155"/>
+      <c r="AM41" s="155"/>
+      <c r="AN41" s="155"/>
+      <c r="AO41" s="155"/>
+      <c r="AP41" s="155"/>
+      <c r="AQ41" s="155"/>
+      <c r="AR41" s="155"/>
+      <c r="AS41" s="155"/>
+      <c r="AT41" s="155"/>
+      <c r="AU41" s="155"/>
+      <c r="AV41" s="155"/>
+      <c r="AW41" s="155"/>
+      <c r="AX41" s="155"/>
+      <c r="AY41" s="155"/>
+      <c r="AZ41" s="155"/>
+      <c r="BA41" s="155"/>
+      <c r="BB41" s="155"/>
+      <c r="BC41" s="155"/>
+      <c r="BD41" s="155"/>
+      <c r="BE41" s="155"/>
+      <c r="BF41" s="155"/>
+      <c r="BG41" s="155"/>
+      <c r="BH41" s="155"/>
+      <c r="BI41" s="155"/>
+      <c r="BJ41" s="155"/>
+      <c r="BK41" s="155"/>
+      <c r="BL41" s="155"/>
+      <c r="BM41" s="155"/>
+      <c r="BN41" s="155"/>
+      <c r="BO41" s="155"/>
+      <c r="BP41" s="155"/>
+      <c r="BQ41" s="155"/>
+      <c r="BR41" s="155"/>
+      <c r="BS41" s="155"/>
+      <c r="BT41" s="155"/>
+      <c r="BU41" s="155"/>
+      <c r="BV41" s="155"/>
+    </row>
+    <row r="42" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A42" s="151"/>
+      <c r="B42" s="157" t="s">
+        <v>405</v>
+      </c>
+      <c r="C42" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D42" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E42" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G42" s="157" t="s">
+        <v>375</v>
+      </c>
+      <c r="H42" s="157" t="s">
         <v>422</v>
       </c>
-      <c r="C41" s="88" t="s">
+      <c r="I42" s="151"/>
+      <c r="J42" s="151"/>
+      <c r="K42" s="151"/>
+      <c r="L42" s="151"/>
+      <c r="M42" s="151"/>
+      <c r="N42" s="155"/>
+      <c r="O42" s="155"/>
+      <c r="P42" s="155"/>
+      <c r="Q42" s="155"/>
+      <c r="R42" s="155"/>
+      <c r="S42" s="155"/>
+      <c r="T42" s="155"/>
+      <c r="U42" s="155"/>
+      <c r="V42" s="155"/>
+      <c r="W42" s="155"/>
+      <c r="X42" s="155"/>
+      <c r="Y42" s="155"/>
+      <c r="Z42" s="155"/>
+      <c r="AA42" s="155"/>
+      <c r="AB42" s="155"/>
+      <c r="AC42" s="155"/>
+      <c r="AD42" s="155"/>
+      <c r="AE42" s="155"/>
+      <c r="AF42" s="155"/>
+      <c r="AG42" s="155"/>
+      <c r="AH42" s="155"/>
+      <c r="AI42" s="155"/>
+      <c r="AJ42" s="155"/>
+      <c r="AK42" s="155"/>
+      <c r="AL42" s="155"/>
+      <c r="AM42" s="155"/>
+      <c r="AN42" s="155"/>
+      <c r="AO42" s="155"/>
+      <c r="AP42" s="155"/>
+      <c r="AQ42" s="155"/>
+      <c r="AR42" s="155"/>
+      <c r="AS42" s="155"/>
+      <c r="AT42" s="155"/>
+      <c r="AU42" s="155"/>
+      <c r="AV42" s="155"/>
+      <c r="AW42" s="155"/>
+      <c r="AX42" s="155"/>
+      <c r="AY42" s="155"/>
+      <c r="AZ42" s="155"/>
+      <c r="BA42" s="155"/>
+      <c r="BB42" s="155"/>
+      <c r="BC42" s="155"/>
+      <c r="BD42" s="155"/>
+      <c r="BE42" s="155"/>
+      <c r="BF42" s="155"/>
+      <c r="BG42" s="155"/>
+      <c r="BH42" s="155"/>
+      <c r="BI42" s="155"/>
+      <c r="BJ42" s="155"/>
+      <c r="BK42" s="155"/>
+      <c r="BL42" s="155"/>
+      <c r="BM42" s="155"/>
+      <c r="BN42" s="155"/>
+      <c r="BO42" s="155"/>
+      <c r="BP42" s="155"/>
+      <c r="BQ42" s="155"/>
+      <c r="BR42" s="155"/>
+      <c r="BS42" s="155"/>
+      <c r="BT42" s="155"/>
+      <c r="BU42" s="155"/>
+      <c r="BV42" s="155"/>
+    </row>
+    <row r="43" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A43" s="155"/>
+      <c r="B43" s="157" t="s">
+        <v>411</v>
+      </c>
+      <c r="C43" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="D41" s="88" t="s">
+      <c r="D43" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="E41" s="88" t="s">
+      <c r="E43" s="157" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G41" s="88" t="s">
-        <v>375</v>
-      </c>
-      <c r="H41" s="88" t="s">
+      <c r="F43" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G43" s="157" t="s">
+        <v>238</v>
+      </c>
+      <c r="H43" s="157" t="s">
+        <v>405</v>
+      </c>
+      <c r="I43" s="155"/>
+      <c r="J43" s="155"/>
+      <c r="K43" s="155"/>
+      <c r="L43" s="155"/>
+      <c r="M43" s="155"/>
+      <c r="N43" s="155"/>
+      <c r="O43" s="155"/>
+      <c r="P43" s="155"/>
+      <c r="Q43" s="155"/>
+      <c r="R43" s="155"/>
+      <c r="S43" s="155"/>
+      <c r="T43" s="155"/>
+      <c r="U43" s="155"/>
+      <c r="V43" s="155"/>
+      <c r="W43" s="155"/>
+      <c r="X43" s="155"/>
+      <c r="Y43" s="155"/>
+      <c r="Z43" s="155"/>
+      <c r="AA43" s="155"/>
+      <c r="AB43" s="155"/>
+      <c r="AC43" s="155"/>
+      <c r="AD43" s="155"/>
+      <c r="AE43" s="155"/>
+      <c r="AF43" s="155"/>
+      <c r="AG43" s="155"/>
+      <c r="AH43" s="155"/>
+      <c r="AI43" s="155"/>
+      <c r="AJ43" s="155"/>
+      <c r="AK43" s="155"/>
+      <c r="AL43" s="155"/>
+      <c r="AM43" s="155"/>
+      <c r="AN43" s="155"/>
+      <c r="AO43" s="155"/>
+      <c r="AP43" s="155"/>
+      <c r="AQ43" s="155"/>
+      <c r="AR43" s="155"/>
+      <c r="AS43" s="155"/>
+      <c r="AT43" s="155"/>
+      <c r="AU43" s="155"/>
+      <c r="AV43" s="155"/>
+      <c r="AW43" s="155"/>
+      <c r="AX43" s="155"/>
+      <c r="AY43" s="155"/>
+      <c r="AZ43" s="155"/>
+      <c r="BA43" s="155"/>
+      <c r="BB43" s="155"/>
+      <c r="BC43" s="155"/>
+      <c r="BD43" s="155"/>
+      <c r="BE43" s="155"/>
+      <c r="BF43" s="155"/>
+      <c r="BG43" s="155"/>
+      <c r="BH43" s="155"/>
+      <c r="BI43" s="155"/>
+      <c r="BJ43" s="155"/>
+      <c r="BK43" s="155"/>
+      <c r="BL43" s="155"/>
+      <c r="BM43" s="155"/>
+      <c r="BN43" s="155"/>
+      <c r="BO43" s="155"/>
+      <c r="BP43" s="155"/>
+      <c r="BQ43" s="155"/>
+      <c r="BR43" s="155"/>
+      <c r="BS43" s="155"/>
+      <c r="BT43" s="155"/>
+      <c r="BU43" s="155"/>
+      <c r="BV43" s="155"/>
+    </row>
+    <row r="44" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A44" s="158" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="151" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B45" s="152" t="s">
+        <v>443</v>
+      </c>
+      <c r="C45" s="153"/>
+      <c r="D45" s="153"/>
+    </row>
+    <row r="46" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B46" s="150" t="s">
+        <v>413</v>
+      </c>
+      <c r="C46" s="149" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="149" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" s="149" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="149" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="149" t="s">
+        <v>120</v>
+      </c>
+      <c r="I46" s="149" t="s">
+        <v>119</v>
+      </c>
+      <c r="J46" s="149" t="s">
+        <v>235</v>
+      </c>
+      <c r="K46" s="149" t="s">
+        <v>122</v>
+      </c>
+      <c r="L46" s="149" t="s">
+        <v>121</v>
+      </c>
+      <c r="M46" s="149" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A47" s="155"/>
+      <c r="B47" s="157" t="s">
+        <v>416</v>
+      </c>
+      <c r="C47" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E47" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G47" s="157" t="s">
+        <v>369</v>
+      </c>
+      <c r="H47" s="157">
+        <v>2</v>
+      </c>
+      <c r="I47" s="157" t="s">
+        <v>376</v>
+      </c>
+      <c r="J47" s="157" t="s">
+        <v>416</v>
+      </c>
+      <c r="K47" s="157" t="s">
+        <v>402</v>
+      </c>
+      <c r="L47" s="157" t="s">
+        <v>403</v>
+      </c>
+      <c r="M47" s="157" t="s">
+        <v>416</v>
+      </c>
+      <c r="N47" s="155"/>
+      <c r="O47" s="155"/>
+      <c r="P47" s="155"/>
+      <c r="Q47" s="155"/>
+      <c r="R47" s="155"/>
+      <c r="S47" s="155"/>
+      <c r="T47" s="155"/>
+      <c r="U47" s="155"/>
+      <c r="V47" s="155"/>
+      <c r="W47" s="155"/>
+      <c r="X47" s="155"/>
+      <c r="Y47" s="155"/>
+      <c r="Z47" s="155"/>
+      <c r="AA47" s="155"/>
+      <c r="AB47" s="155"/>
+      <c r="AC47" s="155"/>
+      <c r="AD47" s="155"/>
+      <c r="AE47" s="155"/>
+      <c r="AF47" s="155"/>
+      <c r="AG47" s="155"/>
+      <c r="AH47" s="155"/>
+      <c r="AI47" s="155"/>
+      <c r="AJ47" s="155"/>
+      <c r="AK47" s="155"/>
+      <c r="AL47" s="155"/>
+      <c r="AM47" s="155"/>
+      <c r="AN47" s="155"/>
+      <c r="AO47" s="155"/>
+      <c r="AP47" s="155"/>
+      <c r="AQ47" s="155"/>
+      <c r="AR47" s="155"/>
+      <c r="AS47" s="155"/>
+      <c r="AT47" s="155"/>
+      <c r="AU47" s="155"/>
+      <c r="AV47" s="155"/>
+      <c r="AW47" s="155"/>
+      <c r="AX47" s="155"/>
+      <c r="AY47" s="155"/>
+      <c r="AZ47" s="155"/>
+      <c r="BA47" s="155"/>
+      <c r="BB47" s="155"/>
+      <c r="BC47" s="155"/>
+      <c r="BD47" s="155"/>
+      <c r="BE47" s="155"/>
+      <c r="BF47" s="155"/>
+      <c r="BG47" s="155"/>
+      <c r="BH47" s="155"/>
+      <c r="BI47" s="155"/>
+      <c r="BJ47" s="155"/>
+      <c r="BK47" s="155"/>
+      <c r="BL47" s="155"/>
+      <c r="BM47" s="155"/>
+      <c r="BN47" s="155"/>
+      <c r="BO47" s="155"/>
+      <c r="BP47" s="155"/>
+      <c r="BQ47" s="155"/>
+      <c r="BR47" s="155"/>
+      <c r="BS47" s="155"/>
+      <c r="BT47" s="155"/>
+      <c r="BU47" s="155"/>
+      <c r="BV47" s="155"/>
+    </row>
+    <row r="48" spans="1:74" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B48" s="157" t="s">
+        <v>417</v>
+      </c>
+      <c r="C48" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D48" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E48" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G48" s="157" t="s">
+        <v>372</v>
+      </c>
+      <c r="H48" s="157" t="s">
+        <v>326</v>
+      </c>
+      <c r="I48" s="157" t="s">
+        <v>376</v>
+      </c>
+      <c r="J48" s="157" t="s">
+        <v>417</v>
+      </c>
+      <c r="K48" s="157" t="s">
+        <v>402</v>
+      </c>
+      <c r="L48" s="157" t="s">
+        <v>403</v>
+      </c>
+      <c r="M48" s="157" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="49" spans="1:75" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B49" s="157" t="s">
+        <v>404</v>
+      </c>
+      <c r="C49" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E49" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G49" s="157" t="s">
+        <v>369</v>
+      </c>
+      <c r="H49" s="157" t="s">
+        <v>404</v>
+      </c>
+      <c r="I49" s="157" t="s">
+        <v>376</v>
+      </c>
+      <c r="J49" s="157" t="s">
+        <v>417</v>
+      </c>
+      <c r="K49" s="157" t="s">
+        <v>402</v>
+      </c>
+      <c r="L49" s="157" t="s">
+        <v>403</v>
+      </c>
+      <c r="M49" s="157" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="50" spans="1:75" s="148" customFormat="1">
+      <c r="B50" s="157" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A42" s="93"/>
-      <c r="B42" s="88" t="s">
+      <c r="C50" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D50" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E50" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G50" s="157" t="s">
+        <v>372</v>
+      </c>
+      <c r="H50" s="157" t="s">
+        <v>326</v>
+      </c>
+      <c r="I50" s="157" t="s">
+        <v>377</v>
+      </c>
+      <c r="J50" s="157" t="s">
+        <v>404</v>
+      </c>
+      <c r="K50" s="157" t="s">
+        <v>426</v>
+      </c>
+      <c r="L50" s="157" t="s">
+        <v>427</v>
+      </c>
+      <c r="M50" s="157" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="51" spans="1:75" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B51" s="157" t="s">
         <v>405</v>
       </c>
-      <c r="C42" s="88" t="s">
+      <c r="C51" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="D42" s="88" t="s">
+      <c r="D51" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="E42" s="88" t="s">
+      <c r="E51" s="157" t="s">
         <v>79</v>
       </c>
-      <c r="F42" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G42" s="88" t="s">
-        <v>238</v>
-      </c>
-      <c r="H42" s="88" t="s">
+      <c r="F51" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G51" s="157" t="s">
+        <v>378</v>
+      </c>
+      <c r="H51" s="157" t="s">
+        <v>379</v>
+      </c>
+      <c r="I51" s="157" t="s">
+        <v>380</v>
+      </c>
+      <c r="J51" s="157" t="s">
+        <v>422</v>
+      </c>
+      <c r="K51" s="157" t="s">
+        <v>428</v>
+      </c>
+      <c r="L51" s="157" t="s">
+        <v>429</v>
+      </c>
+      <c r="M51" s="157" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="52" spans="1:75" s="148" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A52" s="155"/>
+      <c r="B52" s="157" t="s">
+        <v>411</v>
+      </c>
+      <c r="C52" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D52" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E52" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G52" s="157" t="s">
+        <v>327</v>
+      </c>
+      <c r="H52" s="157" t="s">
+        <v>562</v>
+      </c>
+      <c r="I52" s="157" t="s">
+        <v>136</v>
+      </c>
+      <c r="J52" s="157" t="s">
         <v>405</v>
       </c>
-      <c r="I42" s="93"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="93"/>
-      <c r="L42" s="93"/>
-      <c r="M42" s="93"/>
-    </row>
-    <row r="43" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="44" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A44" s="94" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="93" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B45" s="96" t="s">
-        <v>443</v>
-      </c>
-      <c r="C45" s="102"/>
-      <c r="D45" s="102"/>
-    </row>
-    <row r="46" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B46" s="87" t="s">
-        <v>413</v>
-      </c>
-      <c r="C46" s="86" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="86" t="s">
-        <v>90</v>
-      </c>
-      <c r="E46" s="86" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" s="86" t="s">
-        <v>117</v>
-      </c>
-      <c r="H46" s="86" t="s">
-        <v>120</v>
-      </c>
-      <c r="I46" s="86" t="s">
-        <v>119</v>
-      </c>
-      <c r="J46" s="86" t="s">
-        <v>235</v>
-      </c>
-      <c r="K46" s="86" t="s">
+      <c r="K52" s="157" t="s">
         <v>122</v>
       </c>
-      <c r="L46" s="86" t="s">
+      <c r="L52" s="157" t="s">
         <v>121</v>
       </c>
-      <c r="M46" s="86" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B47" s="88" t="s">
-        <v>416</v>
-      </c>
-      <c r="C47" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="D47" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="E47" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="F47" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G47" s="88" t="s">
-        <v>369</v>
-      </c>
-      <c r="H47" s="88">
-        <v>2</v>
-      </c>
-      <c r="I47" s="88" t="s">
-        <v>376</v>
-      </c>
-      <c r="J47" s="88" t="s">
-        <v>416</v>
-      </c>
-      <c r="K47" s="88" t="s">
-        <v>402</v>
-      </c>
-      <c r="L47" s="88" t="s">
-        <v>403</v>
-      </c>
-      <c r="M47" s="88" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B48" s="88" t="s">
-        <v>417</v>
-      </c>
-      <c r="C48" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="D48" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="E48" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="F48" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G48" s="88" t="s">
-        <v>369</v>
-      </c>
-      <c r="H48" s="88" t="s">
-        <v>416</v>
-      </c>
-      <c r="I48" s="88" t="s">
-        <v>376</v>
-      </c>
-      <c r="J48" s="88" t="s">
-        <v>417</v>
-      </c>
-      <c r="K48" s="88" t="s">
-        <v>402</v>
-      </c>
-      <c r="L48" s="88" t="s">
-        <v>403</v>
-      </c>
-      <c r="M48" s="88" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B49" s="88" t="s">
-        <v>404</v>
-      </c>
-      <c r="C49" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="D49" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="E49" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="F49" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G49" s="88" t="s">
-        <v>372</v>
-      </c>
-      <c r="H49" s="88" t="s">
-        <v>326</v>
-      </c>
-      <c r="I49" s="88" t="s">
-        <v>377</v>
-      </c>
-      <c r="J49" s="88" t="s">
-        <v>404</v>
-      </c>
-      <c r="K49" s="88" t="s">
-        <v>426</v>
-      </c>
-      <c r="L49" s="88" t="s">
-        <v>427</v>
-      </c>
-      <c r="M49" s="88" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B50" s="88" t="s">
-        <v>422</v>
-      </c>
-      <c r="C50" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="D50" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="E50" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" s="90" t="s">
-        <v>264</v>
-      </c>
-      <c r="G50" s="88" t="s">
-        <v>378</v>
-      </c>
-      <c r="H50" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="I50" s="88" t="s">
-        <v>380</v>
-      </c>
-      <c r="J50" s="88" t="s">
-        <v>422</v>
-      </c>
-      <c r="K50" s="88" t="s">
-        <v>428</v>
-      </c>
-      <c r="L50" s="88" t="s">
-        <v>429</v>
-      </c>
-      <c r="M50" s="88" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" s="84" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B51" s="93"/>
-    </row>
+      <c r="M52" s="157" t="s">
+        <v>563</v>
+      </c>
+      <c r="N52" s="155"/>
+      <c r="O52" s="155"/>
+      <c r="P52" s="155"/>
+      <c r="Q52" s="155"/>
+      <c r="R52" s="155"/>
+      <c r="S52" s="155"/>
+      <c r="T52" s="155"/>
+      <c r="U52" s="155"/>
+      <c r="V52" s="155"/>
+      <c r="W52" s="155"/>
+      <c r="X52" s="155"/>
+      <c r="Y52" s="155"/>
+      <c r="Z52" s="155"/>
+      <c r="AA52" s="155"/>
+      <c r="AB52" s="155"/>
+      <c r="AC52" s="155"/>
+      <c r="AD52" s="155"/>
+      <c r="AE52" s="155"/>
+      <c r="AF52" s="155"/>
+      <c r="AG52" s="155"/>
+      <c r="AH52" s="155"/>
+      <c r="AI52" s="155"/>
+      <c r="AJ52" s="155"/>
+      <c r="AK52" s="155"/>
+      <c r="AL52" s="155"/>
+      <c r="AM52" s="155"/>
+      <c r="AN52" s="155"/>
+      <c r="AO52" s="155"/>
+      <c r="AP52" s="155"/>
+      <c r="AQ52" s="155"/>
+      <c r="AR52" s="155"/>
+      <c r="AS52" s="155"/>
+      <c r="AT52" s="155"/>
+      <c r="AU52" s="155"/>
+      <c r="AV52" s="155"/>
+      <c r="AW52" s="155"/>
+      <c r="AX52" s="155"/>
+      <c r="AY52" s="155"/>
+      <c r="AZ52" s="155"/>
+      <c r="BA52" s="155"/>
+      <c r="BB52" s="155"/>
+      <c r="BC52" s="155"/>
+      <c r="BD52" s="155"/>
+      <c r="BE52" s="155"/>
+      <c r="BF52" s="155"/>
+      <c r="BG52" s="155"/>
+      <c r="BH52" s="155"/>
+      <c r="BI52" s="155"/>
+      <c r="BJ52" s="155"/>
+      <c r="BK52" s="155"/>
+      <c r="BL52" s="155"/>
+      <c r="BM52" s="155"/>
+      <c r="BN52" s="155"/>
+      <c r="BO52" s="155"/>
+      <c r="BP52" s="155"/>
+      <c r="BQ52" s="155"/>
+      <c r="BR52" s="155"/>
+      <c r="BS52" s="155"/>
+      <c r="BT52" s="155"/>
+      <c r="BU52" s="155"/>
+      <c r="BV52" s="155"/>
+      <c r="BW52" s="155"/>
+    </row>
+    <row r="53" spans="1:75" s="148" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="54" spans="1:75" s="148" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="55" spans="1:75" s="148" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="56" spans="1:75" s="148" customFormat="1" ht="12.75" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10064,7 +10586,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -10093,7 +10615,7 @@
         <v>432</v>
       </c>
       <c r="B4" s="92" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="84" customFormat="1"/>
@@ -10102,7 +10624,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="84" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="84" customFormat="1" ht="14.25">
@@ -10110,7 +10632,7 @@
         <v>432</v>
       </c>
       <c r="B7" s="92" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="84" customFormat="1"/>
@@ -10198,8 +10720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BV87"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BU13" sqref="BU13:BU18"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="AZ29" sqref="AZ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -11657,7 +12179,7 @@
         <v>264</v>
       </c>
       <c r="BU15" s="143" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="BV15" s="88">
         <v>1</v>
@@ -11878,7 +12400,7 @@
         <v>264</v>
       </c>
       <c r="BU16" s="143" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="BV16" s="88">
         <v>1</v>
@@ -12099,7 +12621,7 @@
         <v>264</v>
       </c>
       <c r="BU17" s="143" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="BV17" s="88">
         <v>1</v>
@@ -12956,7 +13478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -14965,7 +15487,7 @@
         <v>92</v>
       </c>
       <c r="BU12" s="143" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="BV12" s="11">
         <v>1</v>
@@ -15186,7 +15708,7 @@
         <v>92</v>
       </c>
       <c r="BU13" s="143" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="BV13" s="11">
         <v>1</v>
@@ -15407,7 +15929,7 @@
         <v>92</v>
       </c>
       <c r="BU14" s="143" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="BV14" s="11">
         <v>1</v>
@@ -16109,8 +16631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="E198" sqref="E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -18386,7 +18908,7 @@
         <v>277</v>
       </c>
       <c r="C185" s="33">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D185" s="34" t="s">
         <v>278</v>
@@ -18431,7 +18953,7 @@
         <v>281</v>
       </c>
       <c r="C188" s="33">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D188" s="34" t="s">
         <v>115</v>
@@ -18655,8 +19177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BW54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20432,7 +20954,7 @@
         <v>264</v>
       </c>
       <c r="BU16" s="143" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="BV16" s="88">
         <v>1</v>
@@ -20654,7 +21176,7 @@
         <v>264</v>
       </c>
       <c r="BU17" s="143" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="BV17" s="88">
         <v>1</v>
@@ -20876,7 +21398,7 @@
         <v>264</v>
       </c>
       <c r="BU18" s="143" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="BV18" s="88">
         <v>1</v>
@@ -21910,11 +22432,11 @@
       <c r="B53" s="139" t="s">
         <v>411</v>
       </c>
-      <c r="C53" s="139" t="s">
-        <v>524</v>
-      </c>
-      <c r="D53" s="139" t="s">
-        <v>524</v>
+      <c r="C53" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="D53" s="143" t="s">
+        <v>239</v>
       </c>
       <c r="E53" s="139" t="s">
         <v>79</v>
@@ -21925,8 +22447,8 @@
       <c r="G53" s="139" t="s">
         <v>327</v>
       </c>
-      <c r="H53" s="138" t="s">
-        <v>264</v>
+      <c r="H53" s="143" t="s">
+        <v>562</v>
       </c>
       <c r="I53" s="139" t="s">
         <v>136</v>
@@ -21940,8 +22462,8 @@
       <c r="L53" s="139" t="s">
         <v>121</v>
       </c>
-      <c r="M53" s="139" t="s">
-        <v>525</v>
+      <c r="M53" s="143" t="s">
+        <v>563</v>
       </c>
       <c r="N53" s="140"/>
       <c r="O53" s="140"/>
@@ -27867,10 +28389,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BV136"/>
+  <dimension ref="A1:BW136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BU14" sqref="BU14:BU19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -30028,7 +30550,7 @@
         <v>264</v>
       </c>
       <c r="BU16" s="143" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="BV16" s="68">
         <v>1</v>
@@ -30250,7 +30772,7 @@
         <v>264</v>
       </c>
       <c r="BU17" s="143" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="BV17" s="68">
         <v>1</v>
@@ -30472,7 +30994,7 @@
         <v>264</v>
       </c>
       <c r="BU18" s="143" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="BV18" s="68">
         <v>1</v>
@@ -31842,7 +32364,7 @@
       <c r="BU32" s="64"/>
       <c r="BV32" s="64"/>
     </row>
-    <row r="33" spans="1:13" ht="12.75" customHeight="1">
+    <row r="33" spans="1:74" ht="12.75" customHeight="1">
       <c r="A33" s="72"/>
       <c r="B33" s="68" t="s">
         <v>239</v>
@@ -31871,7 +32393,7 @@
       <c r="L33" s="64"/>
       <c r="M33" s="64"/>
     </row>
-    <row r="34" spans="1:13" ht="12.75" customHeight="1">
+    <row r="34" spans="1:74" ht="12.75" customHeight="1">
       <c r="A34" s="64"/>
       <c r="B34" s="70"/>
       <c r="C34" s="70"/>
@@ -31886,7 +32408,7 @@
       <c r="L34" s="64"/>
       <c r="M34" s="64"/>
     </row>
-    <row r="35" spans="1:13" ht="12.75" customHeight="1">
+    <row r="35" spans="1:74" ht="12.75" customHeight="1">
       <c r="A35" s="71" t="s">
         <v>88</v>
       </c>
@@ -31905,7 +32427,7 @@
       <c r="L35" s="64"/>
       <c r="M35" s="64"/>
     </row>
-    <row r="36" spans="1:13" ht="12.75" customHeight="1">
+    <row r="36" spans="1:74" ht="12.75" customHeight="1">
       <c r="A36" s="64"/>
       <c r="B36" s="73" t="s">
         <v>442</v>
@@ -31926,7 +32448,7 @@
       <c r="L36" s="64"/>
       <c r="M36" s="64"/>
     </row>
-    <row r="37" spans="1:13" ht="12.75" customHeight="1">
+    <row r="37" spans="1:74" ht="12.75" customHeight="1">
       <c r="A37" s="64"/>
       <c r="B37" s="67" t="s">
         <v>413</v>
@@ -31955,7 +32477,7 @@
       <c r="L37" s="64"/>
       <c r="M37" s="64"/>
     </row>
-    <row r="38" spans="1:13" ht="12.75" customHeight="1">
+    <row r="38" spans="1:74" ht="12.75" customHeight="1">
       <c r="A38" s="64"/>
       <c r="B38" s="68" t="s">
         <v>416</v>
@@ -31984,7 +32506,7 @@
       <c r="L38" s="64"/>
       <c r="M38" s="64"/>
     </row>
-    <row r="39" spans="1:13" ht="12.75" customHeight="1">
+    <row r="39" spans="1:74" ht="12.75" customHeight="1">
       <c r="A39" s="64"/>
       <c r="B39" s="68" t="s">
         <v>417</v>
@@ -32013,95 +32535,367 @@
       <c r="L39" s="64"/>
       <c r="M39" s="64"/>
     </row>
-    <row r="40" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A40" s="64"/>
-      <c r="B40" s="68" t="s">
+    <row r="40" spans="1:74" ht="12.75" customHeight="1">
+      <c r="A40" s="155"/>
+      <c r="B40" s="157" t="s">
         <v>404</v>
       </c>
-      <c r="C40" s="68" t="s">
+      <c r="C40" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="D40" s="68" t="s">
+      <c r="D40" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="E40" s="68" t="s">
+      <c r="E40" s="157" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="69" t="s">
-        <v>264</v>
-      </c>
-      <c r="G40" s="68" t="s">
+      <c r="F40" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G40" s="157" t="s">
+        <v>373</v>
+      </c>
+      <c r="H40" s="157" t="s">
+        <v>417</v>
+      </c>
+      <c r="I40" s="155"/>
+      <c r="J40" s="155"/>
+      <c r="K40" s="155"/>
+      <c r="L40" s="155"/>
+      <c r="M40" s="155"/>
+      <c r="N40" s="155"/>
+      <c r="O40" s="155"/>
+      <c r="P40" s="155"/>
+      <c r="Q40" s="155"/>
+      <c r="R40" s="155"/>
+      <c r="S40" s="155"/>
+      <c r="T40" s="155"/>
+      <c r="U40" s="155"/>
+      <c r="V40" s="155"/>
+      <c r="W40" s="155"/>
+      <c r="X40" s="155"/>
+      <c r="Y40" s="155"/>
+      <c r="Z40" s="155"/>
+      <c r="AA40" s="155"/>
+      <c r="AB40" s="155"/>
+      <c r="AC40" s="155"/>
+      <c r="AD40" s="155"/>
+      <c r="AE40" s="155"/>
+      <c r="AF40" s="155"/>
+      <c r="AG40" s="155"/>
+      <c r="AH40" s="155"/>
+      <c r="AI40" s="155"/>
+      <c r="AJ40" s="155"/>
+      <c r="AK40" s="155"/>
+      <c r="AL40" s="155"/>
+      <c r="AM40" s="155"/>
+      <c r="AN40" s="155"/>
+      <c r="AO40" s="155"/>
+      <c r="AP40" s="155"/>
+      <c r="AQ40" s="155"/>
+      <c r="AR40" s="155"/>
+      <c r="AS40" s="155"/>
+      <c r="AT40" s="155"/>
+      <c r="AU40" s="155"/>
+      <c r="AV40" s="155"/>
+      <c r="AW40" s="155"/>
+      <c r="AX40" s="155"/>
+      <c r="AY40" s="155"/>
+      <c r="AZ40" s="155"/>
+      <c r="BA40" s="155"/>
+      <c r="BB40" s="155"/>
+      <c r="BC40" s="155"/>
+      <c r="BD40" s="155"/>
+      <c r="BE40" s="155"/>
+      <c r="BF40" s="155"/>
+      <c r="BG40" s="155"/>
+      <c r="BH40" s="155"/>
+      <c r="BI40" s="155"/>
+      <c r="BJ40" s="155"/>
+      <c r="BK40" s="155"/>
+      <c r="BL40" s="155"/>
+      <c r="BM40" s="155"/>
+      <c r="BN40" s="155"/>
+      <c r="BO40" s="155"/>
+      <c r="BP40" s="155"/>
+      <c r="BQ40" s="155"/>
+      <c r="BR40" s="155"/>
+      <c r="BS40" s="155"/>
+      <c r="BT40" s="155"/>
+      <c r="BU40" s="155"/>
+      <c r="BV40" s="155"/>
+    </row>
+    <row r="41" spans="1:74" ht="12.75" customHeight="1">
+      <c r="A41" s="155"/>
+      <c r="B41" s="157" t="s">
+        <v>422</v>
+      </c>
+      <c r="C41" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D41" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E41" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G41" s="157" t="s">
         <v>374</v>
       </c>
-      <c r="H40" s="68" t="s">
+      <c r="H41" s="157" t="s">
         <v>404</v>
       </c>
-      <c r="I40" s="64"/>
-      <c r="J40" s="64"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="64"/>
-    </row>
-    <row r="41" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A41" s="64"/>
-      <c r="B41" s="68" t="s">
+      <c r="I41" s="155"/>
+      <c r="J41" s="155"/>
+      <c r="K41" s="155"/>
+      <c r="L41" s="155"/>
+      <c r="M41" s="155"/>
+      <c r="N41" s="155"/>
+      <c r="O41" s="155"/>
+      <c r="P41" s="155"/>
+      <c r="Q41" s="155"/>
+      <c r="R41" s="155"/>
+      <c r="S41" s="155"/>
+      <c r="T41" s="155"/>
+      <c r="U41" s="155"/>
+      <c r="V41" s="155"/>
+      <c r="W41" s="155"/>
+      <c r="X41" s="155"/>
+      <c r="Y41" s="155"/>
+      <c r="Z41" s="155"/>
+      <c r="AA41" s="155"/>
+      <c r="AB41" s="155"/>
+      <c r="AC41" s="155"/>
+      <c r="AD41" s="155"/>
+      <c r="AE41" s="155"/>
+      <c r="AF41" s="155"/>
+      <c r="AG41" s="155"/>
+      <c r="AH41" s="155"/>
+      <c r="AI41" s="155"/>
+      <c r="AJ41" s="155"/>
+      <c r="AK41" s="155"/>
+      <c r="AL41" s="155"/>
+      <c r="AM41" s="155"/>
+      <c r="AN41" s="155"/>
+      <c r="AO41" s="155"/>
+      <c r="AP41" s="155"/>
+      <c r="AQ41" s="155"/>
+      <c r="AR41" s="155"/>
+      <c r="AS41" s="155"/>
+      <c r="AT41" s="155"/>
+      <c r="AU41" s="155"/>
+      <c r="AV41" s="155"/>
+      <c r="AW41" s="155"/>
+      <c r="AX41" s="155"/>
+      <c r="AY41" s="155"/>
+      <c r="AZ41" s="155"/>
+      <c r="BA41" s="155"/>
+      <c r="BB41" s="155"/>
+      <c r="BC41" s="155"/>
+      <c r="BD41" s="155"/>
+      <c r="BE41" s="155"/>
+      <c r="BF41" s="155"/>
+      <c r="BG41" s="155"/>
+      <c r="BH41" s="155"/>
+      <c r="BI41" s="155"/>
+      <c r="BJ41" s="155"/>
+      <c r="BK41" s="155"/>
+      <c r="BL41" s="155"/>
+      <c r="BM41" s="155"/>
+      <c r="BN41" s="155"/>
+      <c r="BO41" s="155"/>
+      <c r="BP41" s="155"/>
+      <c r="BQ41" s="155"/>
+      <c r="BR41" s="155"/>
+      <c r="BS41" s="155"/>
+      <c r="BT41" s="155"/>
+      <c r="BU41" s="155"/>
+      <c r="BV41" s="155"/>
+    </row>
+    <row r="42" spans="1:74" ht="12.75" customHeight="1">
+      <c r="A42" s="151"/>
+      <c r="B42" s="157" t="s">
+        <v>405</v>
+      </c>
+      <c r="C42" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D42" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E42" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G42" s="157" t="s">
+        <v>375</v>
+      </c>
+      <c r="H42" s="157" t="s">
         <v>422</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="I42" s="151"/>
+      <c r="J42" s="151"/>
+      <c r="K42" s="151"/>
+      <c r="L42" s="151"/>
+      <c r="M42" s="151"/>
+      <c r="N42" s="155"/>
+      <c r="O42" s="155"/>
+      <c r="P42" s="155"/>
+      <c r="Q42" s="155"/>
+      <c r="R42" s="155"/>
+      <c r="S42" s="155"/>
+      <c r="T42" s="155"/>
+      <c r="U42" s="155"/>
+      <c r="V42" s="155"/>
+      <c r="W42" s="155"/>
+      <c r="X42" s="155"/>
+      <c r="Y42" s="155"/>
+      <c r="Z42" s="155"/>
+      <c r="AA42" s="155"/>
+      <c r="AB42" s="155"/>
+      <c r="AC42" s="155"/>
+      <c r="AD42" s="155"/>
+      <c r="AE42" s="155"/>
+      <c r="AF42" s="155"/>
+      <c r="AG42" s="155"/>
+      <c r="AH42" s="155"/>
+      <c r="AI42" s="155"/>
+      <c r="AJ42" s="155"/>
+      <c r="AK42" s="155"/>
+      <c r="AL42" s="155"/>
+      <c r="AM42" s="155"/>
+      <c r="AN42" s="155"/>
+      <c r="AO42" s="155"/>
+      <c r="AP42" s="155"/>
+      <c r="AQ42" s="155"/>
+      <c r="AR42" s="155"/>
+      <c r="AS42" s="155"/>
+      <c r="AT42" s="155"/>
+      <c r="AU42" s="155"/>
+      <c r="AV42" s="155"/>
+      <c r="AW42" s="155"/>
+      <c r="AX42" s="155"/>
+      <c r="AY42" s="155"/>
+      <c r="AZ42" s="155"/>
+      <c r="BA42" s="155"/>
+      <c r="BB42" s="155"/>
+      <c r="BC42" s="155"/>
+      <c r="BD42" s="155"/>
+      <c r="BE42" s="155"/>
+      <c r="BF42" s="155"/>
+      <c r="BG42" s="155"/>
+      <c r="BH42" s="155"/>
+      <c r="BI42" s="155"/>
+      <c r="BJ42" s="155"/>
+      <c r="BK42" s="155"/>
+      <c r="BL42" s="155"/>
+      <c r="BM42" s="155"/>
+      <c r="BN42" s="155"/>
+      <c r="BO42" s="155"/>
+      <c r="BP42" s="155"/>
+      <c r="BQ42" s="155"/>
+      <c r="BR42" s="155"/>
+      <c r="BS42" s="155"/>
+      <c r="BT42" s="155"/>
+      <c r="BU42" s="155"/>
+      <c r="BV42" s="155"/>
+    </row>
+    <row r="43" spans="1:74" ht="12.75" customHeight="1">
+      <c r="A43" s="155"/>
+      <c r="B43" s="157" t="s">
+        <v>411</v>
+      </c>
+      <c r="C43" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="D41" s="68" t="s">
+      <c r="D43" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="E41" s="68" t="s">
+      <c r="E43" s="157" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="69" t="s">
-        <v>264</v>
-      </c>
-      <c r="G41" s="68" t="s">
-        <v>375</v>
-      </c>
-      <c r="H41" s="68" t="s">
-        <v>422</v>
-      </c>
-      <c r="I41" s="64"/>
-      <c r="J41" s="64"/>
-      <c r="K41" s="64"/>
-      <c r="L41" s="64"/>
-      <c r="M41" s="64"/>
-    </row>
-    <row r="42" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A42" s="70"/>
-      <c r="B42" s="68" t="s">
+      <c r="F43" s="154" t="s">
+        <v>264</v>
+      </c>
+      <c r="G43" s="157" t="s">
+        <v>238</v>
+      </c>
+      <c r="H43" s="157" t="s">
         <v>405</v>
       </c>
-      <c r="C42" s="68" t="s">
-        <v>239</v>
-      </c>
-      <c r="D42" s="68" t="s">
-        <v>239</v>
-      </c>
-      <c r="E42" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="F42" s="69" t="s">
-        <v>264</v>
-      </c>
-      <c r="G42" s="68" t="s">
-        <v>238</v>
-      </c>
-      <c r="H42" s="68" t="s">
-        <v>405</v>
-      </c>
-      <c r="I42" s="70"/>
-      <c r="J42" s="70"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="70"/>
-      <c r="M42" s="70"/>
-    </row>
-    <row r="43" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="44" spans="1:13" ht="12.75" customHeight="1">
+      <c r="I43" s="155"/>
+      <c r="J43" s="155"/>
+      <c r="K43" s="155"/>
+      <c r="L43" s="155"/>
+      <c r="M43" s="155"/>
+      <c r="N43" s="155"/>
+      <c r="O43" s="155"/>
+      <c r="P43" s="155"/>
+      <c r="Q43" s="155"/>
+      <c r="R43" s="155"/>
+      <c r="S43" s="155"/>
+      <c r="T43" s="155"/>
+      <c r="U43" s="155"/>
+      <c r="V43" s="155"/>
+      <c r="W43" s="155"/>
+      <c r="X43" s="155"/>
+      <c r="Y43" s="155"/>
+      <c r="Z43" s="155"/>
+      <c r="AA43" s="155"/>
+      <c r="AB43" s="155"/>
+      <c r="AC43" s="155"/>
+      <c r="AD43" s="155"/>
+      <c r="AE43" s="155"/>
+      <c r="AF43" s="155"/>
+      <c r="AG43" s="155"/>
+      <c r="AH43" s="155"/>
+      <c r="AI43" s="155"/>
+      <c r="AJ43" s="155"/>
+      <c r="AK43" s="155"/>
+      <c r="AL43" s="155"/>
+      <c r="AM43" s="155"/>
+      <c r="AN43" s="155"/>
+      <c r="AO43" s="155"/>
+      <c r="AP43" s="155"/>
+      <c r="AQ43" s="155"/>
+      <c r="AR43" s="155"/>
+      <c r="AS43" s="155"/>
+      <c r="AT43" s="155"/>
+      <c r="AU43" s="155"/>
+      <c r="AV43" s="155"/>
+      <c r="AW43" s="155"/>
+      <c r="AX43" s="155"/>
+      <c r="AY43" s="155"/>
+      <c r="AZ43" s="155"/>
+      <c r="BA43" s="155"/>
+      <c r="BB43" s="155"/>
+      <c r="BC43" s="155"/>
+      <c r="BD43" s="155"/>
+      <c r="BE43" s="155"/>
+      <c r="BF43" s="155"/>
+      <c r="BG43" s="155"/>
+      <c r="BH43" s="155"/>
+      <c r="BI43" s="155"/>
+      <c r="BJ43" s="155"/>
+      <c r="BK43" s="155"/>
+      <c r="BL43" s="155"/>
+      <c r="BM43" s="155"/>
+      <c r="BN43" s="155"/>
+      <c r="BO43" s="155"/>
+      <c r="BP43" s="155"/>
+      <c r="BQ43" s="155"/>
+      <c r="BR43" s="155"/>
+      <c r="BS43" s="155"/>
+      <c r="BT43" s="155"/>
+      <c r="BU43" s="155"/>
+      <c r="BV43" s="155"/>
+    </row>
+    <row r="44" spans="1:74" ht="12.75" customHeight="1">
       <c r="A44" s="71" t="s">
         <v>88</v>
       </c>
@@ -32120,7 +32914,7 @@
       <c r="L44" s="64"/>
       <c r="M44" s="64"/>
     </row>
-    <row r="45" spans="1:13" ht="12.75" customHeight="1">
+    <row r="45" spans="1:74" ht="12.75" customHeight="1">
       <c r="A45" s="64"/>
       <c r="B45" s="73" t="s">
         <v>443</v>
@@ -32137,229 +32931,409 @@
       <c r="L45" s="64"/>
       <c r="M45" s="64"/>
     </row>
-    <row r="46" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A46" s="64"/>
-      <c r="B46" s="67" t="s">
+    <row r="46" spans="1:74" s="141" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B46" s="108" t="s">
         <v>413</v>
       </c>
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="66" t="s">
+      <c r="D46" s="107" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="66" t="s">
+      <c r="E46" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="66" t="s">
+      <c r="F46" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="G46" s="66" t="s">
+      <c r="G46" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="H46" s="66" t="s">
+      <c r="H46" s="107" t="s">
         <v>120</v>
       </c>
-      <c r="I46" s="66" t="s">
+      <c r="I46" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="J46" s="66" t="s">
+      <c r="J46" s="107" t="s">
         <v>235</v>
       </c>
-      <c r="K46" s="66" t="s">
+      <c r="K46" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="L46" s="66" t="s">
+      <c r="L46" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="M46" s="66" t="s">
+      <c r="M46" s="107" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A47" s="64"/>
-      <c r="B47" s="68" t="s">
+    <row r="47" spans="1:74" s="141" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A47" s="146"/>
+      <c r="B47" s="147" t="s">
         <v>416</v>
       </c>
-      <c r="C47" s="68" t="s">
+      <c r="C47" s="147" t="s">
         <v>239</v>
       </c>
-      <c r="D47" s="68" t="s">
+      <c r="D47" s="147" t="s">
         <v>239</v>
       </c>
-      <c r="E47" s="68" t="s">
+      <c r="E47" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="F47" s="69" t="s">
-        <v>264</v>
-      </c>
-      <c r="G47" s="68" t="s">
+      <c r="F47" s="145" t="s">
+        <v>264</v>
+      </c>
+      <c r="G47" s="147" t="s">
         <v>369</v>
       </c>
-      <c r="H47" s="68">
+      <c r="H47" s="147">
         <v>2</v>
       </c>
-      <c r="I47" s="68" t="s">
+      <c r="I47" s="147" t="s">
         <v>376</v>
       </c>
-      <c r="J47" s="68" t="s">
+      <c r="J47" s="147" t="s">
         <v>416</v>
       </c>
-      <c r="K47" s="68" t="s">
+      <c r="K47" s="147" t="s">
         <v>402</v>
       </c>
-      <c r="L47" s="68" t="s">
+      <c r="L47" s="147" t="s">
         <v>403</v>
       </c>
-      <c r="M47" s="68" t="s">
+      <c r="M47" s="147" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A48" s="64"/>
-      <c r="B48" s="68" t="s">
+      <c r="N47" s="146"/>
+      <c r="O47" s="146"/>
+      <c r="P47" s="146"/>
+      <c r="Q47" s="146"/>
+      <c r="R47" s="146"/>
+      <c r="S47" s="146"/>
+      <c r="T47" s="146"/>
+      <c r="U47" s="146"/>
+      <c r="V47" s="146"/>
+      <c r="W47" s="146"/>
+      <c r="X47" s="146"/>
+      <c r="Y47" s="146"/>
+      <c r="Z47" s="146"/>
+      <c r="AA47" s="146"/>
+      <c r="AB47" s="146"/>
+      <c r="AC47" s="146"/>
+      <c r="AD47" s="146"/>
+      <c r="AE47" s="146"/>
+      <c r="AF47" s="146"/>
+      <c r="AG47" s="146"/>
+      <c r="AH47" s="146"/>
+      <c r="AI47" s="146"/>
+      <c r="AJ47" s="146"/>
+      <c r="AK47" s="146"/>
+      <c r="AL47" s="146"/>
+      <c r="AM47" s="146"/>
+      <c r="AN47" s="146"/>
+      <c r="AO47" s="146"/>
+      <c r="AP47" s="146"/>
+      <c r="AQ47" s="146"/>
+      <c r="AR47" s="146"/>
+      <c r="AS47" s="146"/>
+      <c r="AT47" s="146"/>
+      <c r="AU47" s="146"/>
+      <c r="AV47" s="146"/>
+      <c r="AW47" s="146"/>
+      <c r="AX47" s="146"/>
+      <c r="AY47" s="146"/>
+      <c r="AZ47" s="146"/>
+      <c r="BA47" s="146"/>
+      <c r="BB47" s="146"/>
+      <c r="BC47" s="146"/>
+      <c r="BD47" s="146"/>
+      <c r="BE47" s="146"/>
+      <c r="BF47" s="146"/>
+      <c r="BG47" s="146"/>
+      <c r="BH47" s="146"/>
+      <c r="BI47" s="146"/>
+      <c r="BJ47" s="146"/>
+      <c r="BK47" s="146"/>
+      <c r="BL47" s="146"/>
+      <c r="BM47" s="146"/>
+      <c r="BN47" s="146"/>
+      <c r="BO47" s="146"/>
+      <c r="BP47" s="146"/>
+      <c r="BQ47" s="146"/>
+      <c r="BR47" s="146"/>
+      <c r="BS47" s="146"/>
+      <c r="BT47" s="146"/>
+      <c r="BU47" s="146"/>
+      <c r="BV47" s="146"/>
+    </row>
+    <row r="48" spans="1:74" s="141" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B48" s="143" t="s">
         <v>417</v>
       </c>
-      <c r="C48" s="68" t="s">
+      <c r="C48" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="D48" s="68" t="s">
+      <c r="D48" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="E48" s="68" t="s">
+      <c r="E48" s="143" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="69" t="s">
-        <v>264</v>
-      </c>
-      <c r="G48" s="68" t="s">
+      <c r="F48" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="G48" s="143" t="s">
+        <v>372</v>
+      </c>
+      <c r="H48" s="143" t="s">
+        <v>326</v>
+      </c>
+      <c r="I48" s="143" t="s">
+        <v>376</v>
+      </c>
+      <c r="J48" s="143" t="s">
+        <v>417</v>
+      </c>
+      <c r="K48" s="143" t="s">
+        <v>402</v>
+      </c>
+      <c r="L48" s="143" t="s">
+        <v>403</v>
+      </c>
+      <c r="M48" s="143" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="49" spans="1:75" s="141" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B49" s="143" t="s">
+        <v>404</v>
+      </c>
+      <c r="C49" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="E49" s="143" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="G49" s="143" t="s">
         <v>369</v>
       </c>
-      <c r="H48" s="68" t="s">
-        <v>416</v>
-      </c>
-      <c r="I48" s="68" t="s">
+      <c r="H49" s="143" t="s">
+        <v>404</v>
+      </c>
+      <c r="I49" s="143" t="s">
         <v>376</v>
       </c>
-      <c r="J48" s="68" t="s">
+      <c r="J49" s="143" t="s">
         <v>417</v>
       </c>
-      <c r="K48" s="68" t="s">
+      <c r="K49" s="143" t="s">
         <v>402</v>
       </c>
-      <c r="L48" s="68" t="s">
+      <c r="L49" s="143" t="s">
         <v>403</v>
       </c>
-      <c r="M48" s="68" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A49" s="64"/>
-      <c r="B49" s="68" t="s">
+      <c r="M49" s="143" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="50" spans="1:75" s="141" customFormat="1">
+      <c r="B50" s="143" t="s">
+        <v>422</v>
+      </c>
+      <c r="C50" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="D50" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="E50" s="143" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="G50" s="143" t="s">
+        <v>372</v>
+      </c>
+      <c r="H50" s="143" t="s">
+        <v>326</v>
+      </c>
+      <c r="I50" s="143" t="s">
+        <v>377</v>
+      </c>
+      <c r="J50" s="143" t="s">
         <v>404</v>
       </c>
-      <c r="C49" s="68" t="s">
+      <c r="K50" s="143" t="s">
+        <v>426</v>
+      </c>
+      <c r="L50" s="143" t="s">
+        <v>427</v>
+      </c>
+      <c r="M50" s="143" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="51" spans="1:75" s="141" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B51" s="143" t="s">
+        <v>405</v>
+      </c>
+      <c r="C51" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="D49" s="68" t="s">
+      <c r="D51" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="E49" s="68" t="s">
+      <c r="E51" s="143" t="s">
         <v>79</v>
       </c>
-      <c r="F49" s="69" t="s">
-        <v>264</v>
-      </c>
-      <c r="G49" s="68" t="s">
-        <v>372</v>
-      </c>
-      <c r="H49" s="68" t="s">
-        <v>326</v>
-      </c>
-      <c r="I49" s="68" t="s">
-        <v>377</v>
-      </c>
-      <c r="J49" s="68" t="s">
-        <v>404</v>
-      </c>
-      <c r="K49" s="68" t="s">
-        <v>426</v>
-      </c>
-      <c r="L49" s="68" t="s">
-        <v>427</v>
-      </c>
-      <c r="M49" s="68" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A50" s="64"/>
-      <c r="B50" s="68" t="s">
+      <c r="F51" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="G51" s="143" t="s">
+        <v>378</v>
+      </c>
+      <c r="H51" s="143" t="s">
+        <v>379</v>
+      </c>
+      <c r="I51" s="143" t="s">
+        <v>380</v>
+      </c>
+      <c r="J51" s="143" t="s">
         <v>422</v>
       </c>
-      <c r="C50" s="68" t="s">
+      <c r="K51" s="143" t="s">
+        <v>428</v>
+      </c>
+      <c r="L51" s="143" t="s">
+        <v>429</v>
+      </c>
+      <c r="M51" s="143" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="52" spans="1:75" s="141" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A52" s="140"/>
+      <c r="B52" s="143" t="s">
+        <v>411</v>
+      </c>
+      <c r="C52" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="D50" s="68" t="s">
+      <c r="D52" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="E50" s="68" t="s">
+      <c r="E52" s="143" t="s">
         <v>79</v>
       </c>
-      <c r="F50" s="69" t="s">
-        <v>264</v>
-      </c>
-      <c r="G50" s="68" t="s">
-        <v>378</v>
-      </c>
-      <c r="H50" s="68" t="s">
-        <v>379</v>
-      </c>
-      <c r="I50" s="68" t="s">
-        <v>380</v>
-      </c>
-      <c r="J50" s="68" t="s">
-        <v>422</v>
-      </c>
-      <c r="K50" s="68" t="s">
-        <v>428</v>
-      </c>
-      <c r="L50" s="68" t="s">
-        <v>429</v>
-      </c>
-      <c r="M50" s="68" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A51" s="64"/>
-      <c r="B51" s="70"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="64"/>
-      <c r="M51" s="64"/>
-    </row>
-    <row r="52" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="53" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="54" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="55" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="56" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="57" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="58" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="59" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="60" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="61" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="62" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="63" spans="1:13" ht="12.75" customHeight="1"/>
-    <row r="64" spans="1:13" ht="12.75" customHeight="1"/>
+      <c r="F52" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="G52" s="143" t="s">
+        <v>327</v>
+      </c>
+      <c r="H52" s="143" t="s">
+        <v>562</v>
+      </c>
+      <c r="I52" s="143" t="s">
+        <v>136</v>
+      </c>
+      <c r="J52" s="143" t="s">
+        <v>405</v>
+      </c>
+      <c r="K52" s="143" t="s">
+        <v>122</v>
+      </c>
+      <c r="L52" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="M52" s="143" t="s">
+        <v>563</v>
+      </c>
+      <c r="N52" s="140"/>
+      <c r="O52" s="140"/>
+      <c r="P52" s="140"/>
+      <c r="Q52" s="140"/>
+      <c r="R52" s="140"/>
+      <c r="S52" s="140"/>
+      <c r="T52" s="140"/>
+      <c r="U52" s="140"/>
+      <c r="V52" s="140"/>
+      <c r="W52" s="140"/>
+      <c r="X52" s="140"/>
+      <c r="Y52" s="140"/>
+      <c r="Z52" s="140"/>
+      <c r="AA52" s="140"/>
+      <c r="AB52" s="140"/>
+      <c r="AC52" s="140"/>
+      <c r="AD52" s="140"/>
+      <c r="AE52" s="140"/>
+      <c r="AF52" s="140"/>
+      <c r="AG52" s="140"/>
+      <c r="AH52" s="140"/>
+      <c r="AI52" s="140"/>
+      <c r="AJ52" s="140"/>
+      <c r="AK52" s="140"/>
+      <c r="AL52" s="140"/>
+      <c r="AM52" s="140"/>
+      <c r="AN52" s="140"/>
+      <c r="AO52" s="140"/>
+      <c r="AP52" s="140"/>
+      <c r="AQ52" s="140"/>
+      <c r="AR52" s="140"/>
+      <c r="AS52" s="140"/>
+      <c r="AT52" s="140"/>
+      <c r="AU52" s="140"/>
+      <c r="AV52" s="140"/>
+      <c r="AW52" s="140"/>
+      <c r="AX52" s="140"/>
+      <c r="AY52" s="140"/>
+      <c r="AZ52" s="140"/>
+      <c r="BA52" s="140"/>
+      <c r="BB52" s="140"/>
+      <c r="BC52" s="140"/>
+      <c r="BD52" s="140"/>
+      <c r="BE52" s="140"/>
+      <c r="BF52" s="140"/>
+      <c r="BG52" s="140"/>
+      <c r="BH52" s="140"/>
+      <c r="BI52" s="140"/>
+      <c r="BJ52" s="140"/>
+      <c r="BK52" s="140"/>
+      <c r="BL52" s="140"/>
+      <c r="BM52" s="140"/>
+      <c r="BN52" s="140"/>
+      <c r="BO52" s="140"/>
+      <c r="BP52" s="140"/>
+      <c r="BQ52" s="140"/>
+      <c r="BR52" s="140"/>
+      <c r="BS52" s="140"/>
+      <c r="BT52" s="140"/>
+      <c r="BU52" s="140"/>
+      <c r="BV52" s="140"/>
+      <c r="BW52" s="140"/>
+    </row>
+    <row r="53" spans="1:75" s="141" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="54" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="55" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="56" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="57" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="58" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="59" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="60" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="61" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="62" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="63" spans="1:75" ht="12.75" customHeight="1"/>
+    <row r="64" spans="1:75" ht="12.75" customHeight="1"/>
     <row r="65" ht="12.75" customHeight="1"/>
     <row r="66" ht="12.75" customHeight="1"/>
     <row r="67" ht="12.75" customHeight="1"/>

</xml_diff>